<commit_message>
Auto update bond ETF rates
</commit_message>
<xml_diff>
--- a/output/科创债ETF_累计结果.xlsx
+++ b/output/科创债ETF_累计结果.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,6 +474,11 @@
           <t>2025/11/25</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>2025/11/26</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -500,6 +505,9 @@
         <v>59</v>
       </c>
       <c r="H2" t="n">
+        <v>59</v>
+      </c>
+      <c r="I2" t="n">
         <v>59</v>
       </c>
     </row>
@@ -518,6 +526,7 @@
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -546,6 +555,9 @@
       <c r="H4" t="n">
         <v>59</v>
       </c>
+      <c r="I4" t="n">
+        <v>59</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -572,6 +584,9 @@
         <v>59</v>
       </c>
       <c r="H5" t="n">
+        <v>59</v>
+      </c>
+      <c r="I5" t="n">
         <v>59</v>
       </c>
     </row>
@@ -590,6 +605,7 @@
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -606,6 +622,7 @@
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -633,6 +650,9 @@
       </c>
       <c r="H8" t="n">
         <v>60</v>
+      </c>
+      <c r="I8" t="n">
+        <v>59</v>
       </c>
     </row>
     <row r="9">
@@ -650,6 +670,7 @@
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -666,6 +687,7 @@
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -692,6 +714,9 @@
         <v>59</v>
       </c>
       <c r="H11" t="n">
+        <v>59</v>
+      </c>
+      <c r="I11" t="n">
         <v>59</v>
       </c>
     </row>
@@ -710,6 +735,7 @@
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -726,6 +752,7 @@
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -742,6 +769,7 @@
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -768,6 +796,9 @@
         <v>59</v>
       </c>
       <c r="H15" t="n">
+        <v>59</v>
+      </c>
+      <c r="I15" t="n">
         <v>59</v>
       </c>
     </row>
@@ -786,6 +817,7 @@
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -802,6 +834,7 @@
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -818,6 +851,7 @@
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -834,6 +868,7 @@
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -850,6 +885,9 @@
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
+      <c r="I20" t="n">
+        <v>0.6</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -866,6 +904,7 @@
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -882,6 +921,7 @@
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -898,6 +938,9 @@
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr"/>
       <c r="H23" t="inlineStr"/>
+      <c r="I23" t="n">
+        <v>0.6</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -914,6 +957,9 @@
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr"/>
+      <c r="I24" t="n">
+        <v>0.59</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -930,6 +976,9 @@
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr"/>
+      <c r="I25" t="n">
+        <v>0.59</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>